<commit_message>
10-08-2022 add fix in kug
</commit_message>
<xml_diff>
--- a/templates/template_KUG.xlsx
+++ b/templates/template_KUG.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\localhost\docs\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenServer\OpenServer\domains\localhost\docs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC403E5-58A0-499D-A928-676353507179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,18 +133,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -156,18 +164,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -447,76 +462,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="35.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="1" t="s">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="2" t="s">
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="6" t="s">
+    <row r="4" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="8" t="s">
+    <row r="6" spans="1:7" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="11" spans="1:7" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -525,7 +540,7 @@
       <c r="C11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -537,6 +552,9 @@
       <c r="G11" s="11" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -548,5 +566,6 @@
     <mergeCell ref="C9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>